<commit_message>
pay merchant with voucher code
</commit_message>
<xml_diff>
--- a/FolderExcelFiles/I - SUBCRIBER/3. Transactions/transfer/transfer to mobile/2.1 Transfer - To - Mobile - Fail 2.xlsx
+++ b/FolderExcelFiles/I - SUBCRIBER/3. Transactions/transfer/transfer to mobile/2.1 Transfer - To - Mobile - Fail 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\AYA Subscriber App\FolderExcelFiles\I - SUBCRIBER\3. Transactions\transfer\transfer to mobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9994FB94-4B3D-4F90-B5B2-0C7F4EA6850B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ED8FDD-91D4-4BB7-90A3-760295BE20C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1432A72A-0386-441C-9E35-C35EB92B75C6}"/>
+    <workbookView xWindow="1110" yWindow="2655" windowWidth="27255" windowHeight="12675" xr2:uid="{1432A72A-0386-441C-9E35-C35EB92B75C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA4BE065-FC04-4F51-9602-B7E638619A1A}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
         <v>19</v>
       </c>
       <c r="M2" t="str">
-        <f>B2</f>
+        <f t="shared" ref="M2:M7" si="0">B2</f>
         <v>000000</v>
       </c>
       <c r="N2">
@@ -684,7 +684,7 @@
         <v>19</v>
       </c>
       <c r="M3" t="str">
-        <f>B3</f>
+        <f t="shared" si="0"/>
         <v>000000</v>
       </c>
       <c r="N3">
@@ -736,7 +736,7 @@
         <v>19</v>
       </c>
       <c r="M4" t="str">
-        <f>B4</f>
+        <f t="shared" si="0"/>
         <v>000000</v>
       </c>
       <c r="N4">
@@ -788,7 +788,7 @@
         <v>19</v>
       </c>
       <c r="M5" t="str">
-        <f>B5</f>
+        <f t="shared" si="0"/>
         <v>000000</v>
       </c>
       <c r="N5">
@@ -840,7 +840,7 @@
         <v>19</v>
       </c>
       <c r="M6" t="str">
-        <f>B6</f>
+        <f t="shared" si="0"/>
         <v>000000</v>
       </c>
       <c r="N6">
@@ -892,7 +892,7 @@
         <v>34</v>
       </c>
       <c r="M7" t="str">
-        <f>B7</f>
+        <f t="shared" si="0"/>
         <v>000000</v>
       </c>
       <c r="N7">

</xml_diff>